<commit_message>
Se dividen los escenarios a nivel de feauture, se estabiliza el banner, se cambia la autenticacion
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="7425" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7695" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
     <t>MasterCard</t>
   </si>
   <si>
-    <t>5306950634968354</t>
+    <t>5306 9506 3496 8354</t>
   </si>
   <si>
     <t>zrediseño12</t>
@@ -166,10 +166,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -209,6 +209,128 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,128 +345,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -373,25 +373,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,7 +475,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -415,145 +517,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -582,22 +582,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -627,36 +622,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -679,152 +644,187 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1312,7 +1312,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>

</xml_diff>

<commit_message>
consulta detalle e-prepago a el log del canal
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUTOMATIZACION JAVA\PROYECTOS GRADLE\PROYECTOS NUEVA APP\AW1059001_APPSucursalVirtualPersonas_Test\APP_PERSONAS\src\test\resources\datadriven\consultas\detalleproductos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilo_betancur_hernandez/Documents/AW1059001_APPSucursalVirtualPersonas_Test/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A6548E-CB4C-8640-885C-389A83CA62A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19890" windowHeight="7425"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19900" windowHeight="7420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -164,18 +165,37 @@
   </si>
   <si>
     <t>Consultas</t>
+  </si>
+  <si>
+    <t>userrobot4</t>
+  </si>
+  <si>
+    <t>5306953604979344</t>
+  </si>
+  <si>
+    <t>22452521</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -253,26 +273,29 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -544,23 +567,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P4" sqref="O4:P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
-    <col min="13" max="13" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -649,6 +672,188 @@
       </c>
       <c r="N2" s="11" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="5"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N4"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -685,7 +890,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -697,22 +902,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="M2" sqref="M2:O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -770,7 +975,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>17</v>
@@ -796,12 +1001,8 @@
       <c r="L2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>28</v>
-      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="5"/>
@@ -837,7 +1038,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -849,22 +1050,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -922,7 +1123,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>17</v>
@@ -985,155 +1186,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Listas!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:J4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="5"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$3</xm:f>
           </x14:formula1>
@@ -1146,19 +1199,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
se crean detalles de transacciones y modificacion de data
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20130" windowHeight="7425" activeTab="3"/>
+    <workbookView windowWidth="20490" windowHeight="7695" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -119,7 +119,10 @@
     <t>invictus10</t>
   </si>
   <si>
-    <t>zrediseño12</t>
+    <t>****9344</t>
+  </si>
+  <si>
+    <t>Préstamo</t>
   </si>
   <si>
     <t>Tarjeta de crédito</t>
@@ -181,9 +184,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -211,6 +214,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -218,7 +228,68 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,6 +303,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -240,14 +350,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -255,111 +357,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -388,43 +391,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,139 +571,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -597,17 +600,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -644,17 +641,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -663,8 +653,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -686,160 +676,173 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -862,55 +865,55 @@
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Título 3" xfId="1" builtinId="18"/>
-    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
-    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
-    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Moneda" xfId="5" builtinId="4"/>
-    <cellStyle name="Coma" xfId="6" builtinId="3"/>
-    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
-    <cellStyle name="Hipervínculo" xfId="8" builtinId="8"/>
-    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21"/>
-    <cellStyle name="Nota" xfId="11" builtinId="10"/>
-    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
-    <cellStyle name="Texto de advertencia" xfId="13" builtinId="11"/>
-    <cellStyle name="Título" xfId="14" builtinId="15"/>
-    <cellStyle name="Texto explicativo" xfId="15" builtinId="53"/>
-    <cellStyle name="Título 1" xfId="16" builtinId="16"/>
-    <cellStyle name="Título 4" xfId="17" builtinId="19"/>
-    <cellStyle name="Entrada" xfId="18" builtinId="20"/>
-    <cellStyle name="Cálculo" xfId="19" builtinId="22"/>
-    <cellStyle name="Celda de comprobación" xfId="20" builtinId="23"/>
-    <cellStyle name="Celda vinculada" xfId="21" builtinId="24"/>
-    <cellStyle name="Total" xfId="22" builtinId="25"/>
-    <cellStyle name="Correcto" xfId="23" builtinId="26"/>
-    <cellStyle name="40% - Énfasis5" xfId="24" builtinId="47"/>
-    <cellStyle name="Incorrecto" xfId="25" builtinId="27"/>
-    <cellStyle name="Neutro" xfId="26" builtinId="28"/>
-    <cellStyle name="20% - Énfasis5" xfId="27" builtinId="46"/>
-    <cellStyle name="Énfasis1" xfId="28" builtinId="29"/>
-    <cellStyle name="20% - Énfasis1" xfId="29" builtinId="30"/>
-    <cellStyle name="60% - Énfasis1" xfId="30" builtinId="32"/>
-    <cellStyle name="20% - Énfasis6" xfId="31" builtinId="50"/>
-    <cellStyle name="Énfasis2" xfId="32" builtinId="33"/>
-    <cellStyle name="20% - Énfasis2" xfId="33" builtinId="34"/>
-    <cellStyle name="40% - Énfasis2" xfId="34" builtinId="35"/>
-    <cellStyle name="60% - Énfasis2" xfId="35" builtinId="36"/>
-    <cellStyle name="Énfasis3" xfId="36" builtinId="37"/>
-    <cellStyle name="20% - Énfasis3" xfId="37" builtinId="38"/>
-    <cellStyle name="40% - Énfasis3" xfId="38" builtinId="39"/>
-    <cellStyle name="60% - Énfasis3" xfId="39" builtinId="40"/>
-    <cellStyle name="Énfasis4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Énfasis4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Énfasis4" xfId="42" builtinId="43"/>
-    <cellStyle name="60% - Énfasis4" xfId="43" builtinId="44"/>
-    <cellStyle name="Énfasis5" xfId="44" builtinId="45"/>
-    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48"/>
-    <cellStyle name="Énfasis6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
-    <cellStyle name="Normal 2" xfId="48"/>
-    <cellStyle name="60% - Énfasis6" xfId="49" builtinId="52"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="Normal 2" xfId="32"/>
+    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="40" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="41" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="43" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="44" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="45" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="46" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="47" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="48" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="49" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1360,8 +1363,8 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
@@ -1459,7 +1462,7 @@
         <v>30</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1507,8 +1510,8 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:O2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
@@ -1519,6 +1522,7 @@
     <col min="10" max="10" width="22.1666666666667" customWidth="1"/>
     <col min="11" max="11" width="14.3333333333333" customWidth="1"/>
     <col min="12" max="12" width="14.6666666666667" customWidth="1"/>
+    <col min="14" max="14" width="12.625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1576,7 +1580,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>17</v>
@@ -1602,8 +1606,12 @@
       <c r="L2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="M2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="3">
+        <v>29281023956</v>
+      </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="5"/>
@@ -1650,7 +1658,7 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -1746,10 +1754,10 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1811,16 +1819,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1828,50 +1836,50 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifican excel para data en ejecucion
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695" activeTab="2"/>
+    <workbookView windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -68,7 +68,7 @@
     <t>1037655531</t>
   </si>
   <si>
-    <t>userrobot3</t>
+    <t>invictus10</t>
   </si>
   <si>
     <t>1234</t>
@@ -98,7 +98,7 @@
     <t>Corriente</t>
   </si>
   <si>
-    <t>406-101390-08</t>
+    <t>406-125210-00</t>
   </si>
   <si>
     <t>2</t>
@@ -107,16 +107,13 @@
     <t>22452521</t>
   </si>
   <si>
-    <t>userrobot4</t>
+    <t>Ahorros</t>
+  </si>
+  <si>
+    <t>406-725210-12</t>
   </si>
   <si>
     <t>MasterCard</t>
-  </si>
-  <si>
-    <t>*9344</t>
-  </si>
-  <si>
-    <t>invictus10</t>
   </si>
   <si>
     <t>****9344</t>
@@ -184,10 +181,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -214,16 +211,24 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -249,6 +254,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -258,14 +270,76 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,83 +360,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -391,187 +388,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,6 +593,15 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -641,20 +647,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -676,173 +686,160 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1184,8 +1181,8 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
@@ -1299,7 +1296,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>17</v>
@@ -1326,10 +1323,10 @@
         <v>24</v>
       </c>
       <c r="M3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="14" t="s">
         <v>30</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1363,7 +1360,7 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -1432,7 +1429,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>17</v>
@@ -1459,10 +1456,10 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1510,7 +1507,7 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
@@ -1580,7 +1577,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>17</v>
@@ -1607,7 +1604,7 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N2" s="3">
         <v>29281023956</v>
@@ -1658,7 +1655,7 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -1727,7 +1724,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>17</v>
@@ -1754,10 +1751,10 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1819,16 +1816,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1836,50 +1833,50 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
         <v>44</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
         <v>48</v>
-      </c>
-      <c r="D4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mapeo para realizar consulta de detalle de productos
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,12 @@
     <sheet name="TarjetasCredito" sheetId="4" r:id="rId4"/>
     <sheet name="Listas" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -119,15 +129,6 @@
     <t>****9344</t>
   </si>
   <si>
-    <t>Préstamo</t>
-  </si>
-  <si>
-    <t>Tarjeta de crédito</t>
-  </si>
-  <si>
-    <t>*6682</t>
-  </si>
-  <si>
     <t>Orientacion</t>
   </si>
   <si>
@@ -174,24 +175,34 @@
   </si>
   <si>
     <t>Consultas</t>
+  </si>
+  <si>
+    <t>Personal American Express</t>
+  </si>
+  <si>
+    <t>*7806</t>
+  </si>
+  <si>
+    <t>Prestamo personal ta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -209,159 +220,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,194 +246,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -596,322 +270,33 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Título 3" xfId="1" builtinId="18"/>
-    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
-    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
-    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Moneda" xfId="5" builtinId="4"/>
-    <cellStyle name="Coma" xfId="6" builtinId="3"/>
-    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
-    <cellStyle name="Hipervínculo" xfId="8" builtinId="8"/>
-    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21"/>
-    <cellStyle name="Nota" xfId="11" builtinId="10"/>
-    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
-    <cellStyle name="Texto de advertencia" xfId="13" builtinId="11"/>
-    <cellStyle name="Título" xfId="14" builtinId="15"/>
-    <cellStyle name="Texto explicativo" xfId="15" builtinId="53"/>
-    <cellStyle name="Título 1" xfId="16" builtinId="16"/>
-    <cellStyle name="Título 4" xfId="17" builtinId="19"/>
-    <cellStyle name="Entrada" xfId="18" builtinId="20"/>
-    <cellStyle name="Cálculo" xfId="19" builtinId="22"/>
-    <cellStyle name="Celda de comprobación" xfId="20" builtinId="23"/>
-    <cellStyle name="Celda vinculada" xfId="21" builtinId="24"/>
-    <cellStyle name="Total" xfId="22" builtinId="25"/>
-    <cellStyle name="Correcto" xfId="23" builtinId="26"/>
-    <cellStyle name="40% - Énfasis5" xfId="24" builtinId="47"/>
-    <cellStyle name="Incorrecto" xfId="25" builtinId="27"/>
-    <cellStyle name="Neutro" xfId="26" builtinId="28"/>
-    <cellStyle name="20% - Énfasis5" xfId="27" builtinId="46"/>
-    <cellStyle name="Énfasis1" xfId="28" builtinId="29"/>
-    <cellStyle name="20% - Énfasis1" xfId="29" builtinId="30"/>
-    <cellStyle name="60% - Énfasis1" xfId="30" builtinId="32"/>
-    <cellStyle name="20% - Énfasis6" xfId="31" builtinId="50"/>
-    <cellStyle name="Énfasis2" xfId="32" builtinId="33"/>
-    <cellStyle name="20% - Énfasis2" xfId="33" builtinId="34"/>
-    <cellStyle name="40% - Énfasis2" xfId="34" builtinId="35"/>
-    <cellStyle name="60% - Énfasis2" xfId="35" builtinId="36"/>
-    <cellStyle name="Énfasis3" xfId="36" builtinId="37"/>
-    <cellStyle name="20% - Énfasis3" xfId="37" builtinId="38"/>
-    <cellStyle name="40% - Énfasis3" xfId="38" builtinId="39"/>
-    <cellStyle name="60% - Énfasis3" xfId="39" builtinId="40"/>
-    <cellStyle name="Énfasis4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Énfasis4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Énfasis4" xfId="42" builtinId="43"/>
-    <cellStyle name="60% - Énfasis4" xfId="43" builtinId="44"/>
-    <cellStyle name="Énfasis5" xfId="44" builtinId="45"/>
-    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48"/>
-    <cellStyle name="Énfasis6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
-    <cellStyle name="Normal 2" xfId="48"/>
-    <cellStyle name="60% - Énfasis6" xfId="49" builtinId="52"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1173,31 +558,31 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1666666666667" customWidth="1"/>
-    <col min="2" max="6" width="14.3333333333333" customWidth="1"/>
-    <col min="9" max="9" width="18.3333333333333" customWidth="1"/>
-    <col min="10" max="10" width="22.1666666666667" customWidth="1"/>
-    <col min="11" max="11" width="14.3333333333333" customWidth="1"/>
-    <col min="12" max="12" width="14.6666666666667" customWidth="1"/>
-    <col min="13" max="13" width="10.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1241,7 +626,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>14</v>
       </c>
@@ -1285,7 +670,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>27</v>
       </c>
@@ -1329,7 +714,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1344,37 +729,42 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1666666666667" customWidth="1"/>
-    <col min="2" max="6" width="14.3333333333333" customWidth="1"/>
-    <col min="9" max="9" width="18.3333333333333" customWidth="1"/>
-    <col min="10" max="10" width="22.1666666666667" customWidth="1"/>
-    <col min="11" max="11" width="14.3333333333333" customWidth="1"/>
-    <col min="12" max="12" width="14.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1418,7 +808,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>14</v>
       </c>
@@ -1462,7 +852,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1476,7 +866,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1491,38 +881,43 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1666666666667" customWidth="1"/>
-    <col min="2" max="6" width="14.3333333333333" customWidth="1"/>
-    <col min="9" max="9" width="18.3333333333333" customWidth="1"/>
-    <col min="10" max="10" width="22.1666666666667" customWidth="1"/>
-    <col min="11" max="11" width="14.3333333333333" customWidth="1"/>
-    <col min="12" max="12" width="14.6666666666667" customWidth="1"/>
-    <col min="14" max="14" width="12.625"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1566,7 +961,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>14</v>
       </c>
@@ -1604,13 +999,13 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="N2" s="3">
         <v>29281023956</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1624,7 +1019,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1639,37 +1034,42 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1666666666667" customWidth="1"/>
-    <col min="2" max="6" width="14.3333333333333" customWidth="1"/>
-    <col min="9" max="9" width="18.3333333333333" customWidth="1"/>
-    <col min="10" max="10" width="22.1666666666667" customWidth="1"/>
-    <col min="11" max="11" width="14.3333333333333" customWidth="1"/>
-    <col min="12" max="12" width="14.6666666666667" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="6" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1713,7 +1113,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>14</v>
       </c>
@@ -1751,13 +1151,13 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1771,7 +1171,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1786,101 +1186,105 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="14.8333333333333" customWidth="1"/>
-    <col min="3" max="3" width="12.1666666666667" customWidth="1"/>
-    <col min="4" max="4" width="17.8333333333333" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>40</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>44</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
-      <c r="B4" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>47</v>
       </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
-      <c r="B5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2">
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2">
-      <c r="B7" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Creación de consulta detalle eprepago
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -127,9 +127,6 @@
     <t>MasterCard</t>
   </si>
   <si>
-    <t>****9344</t>
-  </si>
-  <si>
     <t>Orientacion</t>
   </si>
   <si>
@@ -185,6 +182,15 @@
   </si>
   <si>
     <t>Prestamo personal ta</t>
+  </si>
+  <si>
+    <t>pruebauser01</t>
+  </si>
+  <si>
+    <t>6789</t>
+  </si>
+  <si>
+    <t>****0252</t>
   </si>
 </sst>
 </file>
@@ -751,8 +757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -820,10 +826,10 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>18</v>
@@ -850,7 +856,7 @@
         <v>31</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -1000,7 +1006,7 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N2" s="3">
         <v>29281023956</v>
@@ -1056,7 +1062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -1255,10 +1261,10 @@
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -1325,16 +1331,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1342,50 +1348,50 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
         <v>40</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>41</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>42</v>
-      </c>
-      <c r="D3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
         <v>44</v>
-      </c>
-      <c r="D4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se crea POC con gmail
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7695" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Crediagil" sheetId="6" r:id="rId4"/>
     <sheet name="TarjetasCredito" sheetId="4" r:id="rId5"/>
     <sheet name="Listas" sheetId="2" r:id="rId6"/>
+    <sheet name="EprepagoPOC" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -172,6 +173,30 @@
   </si>
   <si>
     <t>Consultas</t>
+  </si>
+  <si>
+    <t>nombrePersonalizado</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>tipoCorreo</t>
+  </si>
+  <si>
+    <t>numeroCelular</t>
+  </si>
+  <si>
+    <t>invictusdiez</t>
+  </si>
+  <si>
+    <t>automatizaciontodo1@gmail.com</t>
+  </si>
+  <si>
+    <t>Laboral</t>
+  </si>
+  <si>
+    <t>3145678956</t>
   </si>
 </sst>
 </file>
@@ -181,10 +206,10 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -209,14 +234,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -230,6 +256,105 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -238,6 +363,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,77 +379,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -329,37 +391,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,6 +413,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -392,186 +431,186 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -595,12 +634,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -621,10 +664,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -641,6 +682,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -686,172 +736,181 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
@@ -1232,30 +1291,30 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="20" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1264,42 +1323,42 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="20" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="19" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="20" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1308,38 +1367,38 @@
       <c r="H3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="21" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="5"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1358,8 +1417,8 @@
   <sheetPr/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="A1:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
@@ -1409,21 +1468,21 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="3">
         <v>1037655531</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1432,7 +1491,7 @@
       <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="20" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1441,16 +1500,16 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="20" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -1461,32 +1520,32 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="5"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1557,30 +1616,30 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="20" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1589,16 +1648,16 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="20" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -1609,32 +1668,32 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="5"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1698,22 +1757,22 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="20" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1722,16 +1781,16 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="20" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1802,30 +1861,30 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="20" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1834,16 +1893,16 @@
       <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="7" t="s">
         <v>21</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="20" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -1854,32 +1913,32 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="5"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1979,4 +2038,166 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:R3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1" width="3.25" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="3" max="3" width="15.375" customWidth="1"/>
+    <col min="4" max="4" width="10.125" customWidth="1"/>
+    <col min="5" max="5" width="6.125" customWidth="1"/>
+    <col min="6" max="6" width="14.625" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="12.25" customWidth="1"/>
+    <col min="9" max="10" width="19.125" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="12" max="12" width="12.75" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="14.625" customWidth="1"/>
+    <col min="15" max="15" width="22" customWidth="1"/>
+    <col min="16" max="16" width="29.375" customWidth="1"/>
+    <col min="17" max="17" width="11.125" customWidth="1"/>
+    <col min="18" max="18" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3">
+        <v>22452521</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="15:18">
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J2">
+      <formula1>Listas!$A$2:$A$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="P2" r:id="rId1" display="automatizaciontodo1@gmail.com" tooltip="mailto:automatizaciontodo1@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se estabiliza lectura de clave dinamica por gmail para Android
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositorios TODO1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\consultas\detalleproductos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17CDB41-E4D0-4599-A430-37979FD071FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695" activeTab="6"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="60">
   <si>
     <t>ID</t>
   </si>
@@ -197,19 +203,16 @@
   </si>
   <si>
     <t>3145678956</t>
+  </si>
+  <si>
+    <t>autotest30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -248,151 +251,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="37">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -423,194 +296,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -646,254 +333,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -903,7 +351,7 @@
     <xf numFmtId="49" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -913,66 +361,23 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="Normal 2" xfId="32"/>
-    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="40" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="41" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="43" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="44" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="45" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="46" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="47" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="48" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="49" builtinId="52"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1230,27 +635,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
-    <col min="13" max="13" width="10.375" customWidth="1"/>
+    <col min="1" max="1" width="11.09765625" customWidth="1"/>
+    <col min="2" max="6" width="14.3984375" customWidth="1"/>
+    <col min="9" max="9" width="18.3984375" customWidth="1"/>
+    <col min="10" max="10" width="22.09765625" customWidth="1"/>
+    <col min="11" max="11" width="14.3984375" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" customWidth="1"/>
+    <col min="13" max="13" width="10.3984375" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1386,7 +791,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="13"/>
       <c r="B4" s="15"/>
       <c r="C4" s="13"/>
@@ -1401,34 +806,39 @@
       <c r="L4" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N2" sqref="A1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.09765625" customWidth="1"/>
+    <col min="2" max="6" width="14.3984375" customWidth="1"/>
+    <col min="9" max="9" width="18.3984375" customWidth="1"/>
+    <col min="10" max="10" width="22.09765625" customWidth="1"/>
+    <col min="11" max="11" width="14.3984375" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1519,7 +929,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="14"/>
@@ -1533,7 +943,7 @@
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="13"/>
       <c r="B4" s="15"/>
       <c r="C4" s="13"/>
@@ -1548,35 +958,40 @@
       <c r="L4" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:N2"/>
+      <selection sqref="A1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
-    <col min="14" max="14" width="12.125" customWidth="1"/>
+    <col min="1" max="1" width="11.09765625" customWidth="1"/>
+    <col min="2" max="6" width="14.3984375" customWidth="1"/>
+    <col min="9" max="9" width="18.3984375" customWidth="1"/>
+    <col min="10" max="10" width="22.09765625" customWidth="1"/>
+    <col min="11" max="11" width="14.3984375" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" customWidth="1"/>
+    <col min="14" max="14" width="12.09765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1667,7 +1082,7 @@
         <v>29281023956</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="14"/>
@@ -1681,7 +1096,7 @@
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="13"/>
       <c r="B4" s="15"/>
       <c r="C4" s="13"/>
@@ -1696,27 +1111,32 @@
       <c r="L4" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
@@ -1795,33 +1215,38 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J2">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="6" width="14.375" customWidth="1"/>
-    <col min="9" max="9" width="18.375" customWidth="1"/>
-    <col min="10" max="10" width="22.125" customWidth="1"/>
-    <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="11.09765625" customWidth="1"/>
+    <col min="2" max="6" width="14.3984375" customWidth="1"/>
+    <col min="9" max="9" width="18.3984375" customWidth="1"/>
+    <col min="10" max="10" width="22.09765625" customWidth="1"/>
+    <col min="11" max="11" width="14.3984375" customWidth="1"/>
+    <col min="12" max="12" width="14.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1912,7 +1337,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="14"/>
@@ -1926,7 +1351,7 @@
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="13"/>
       <c r="B4" s="15"/>
       <c r="C4" s="13"/>
@@ -1941,32 +1366,37 @@
       <c r="L4" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="14.875" customWidth="1"/>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
+    <col min="1" max="1" width="10.59765625" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" customWidth="1"/>
+    <col min="3" max="3" width="12.09765625" customWidth="1"/>
+    <col min="4" max="4" width="17.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2011,7 +1441,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>46</v>
       </c>
@@ -2019,54 +1449,52 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="1:4">
       <c r="B5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="1:4">
       <c r="B6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="3.25" customWidth="1"/>
-    <col min="2" max="2" width="19.125" customWidth="1"/>
-    <col min="3" max="3" width="15.375" customWidth="1"/>
-    <col min="4" max="4" width="10.125" customWidth="1"/>
-    <col min="5" max="5" width="6.125" customWidth="1"/>
-    <col min="6" max="6" width="14.625" customWidth="1"/>
+    <col min="1" max="1" width="3.19921875" customWidth="1"/>
+    <col min="2" max="2" width="19.09765625" customWidth="1"/>
+    <col min="3" max="3" width="15.3984375" customWidth="1"/>
+    <col min="4" max="4" width="10.09765625" customWidth="1"/>
+    <col min="5" max="5" width="6.09765625" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" customWidth="1"/>
     <col min="7" max="7" width="11.5" customWidth="1"/>
-    <col min="8" max="8" width="12.25" customWidth="1"/>
-    <col min="9" max="10" width="19.125" customWidth="1"/>
+    <col min="8" max="8" width="12.19921875" customWidth="1"/>
+    <col min="9" max="10" width="19.09765625" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="12.75" customWidth="1"/>
+    <col min="12" max="12" width="12.69921875" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="14.625" customWidth="1"/>
+    <col min="14" max="14" width="14.59765625" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
-    <col min="16" max="16" width="29.375" customWidth="1"/>
-    <col min="17" max="17" width="11.125" customWidth="1"/>
+    <col min="16" max="16" width="29.3984375" customWidth="1"/>
+    <col min="17" max="17" width="11.09765625" customWidth="1"/>
     <col min="18" max="18" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2137,7 +1565,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>17</v>
@@ -2182,22 +1610,28 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="15:18">
+    <row r="3" spans="1:18">
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J2">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="P2" r:id="rId1" display="automatizaciontodo1@gmail.com" tooltip="mailto:automatizaciontodo1@gmail.com"/>
+    <hyperlink ref="P2" r:id="rId1" tooltip="mailto:automatizaciontodo1@gmail.com" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000000000000}">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correcion automatizacion para ejecucion
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/consultas/detalleproductos/ConsultaDetalleProductos.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TODO1\OSP_NEW\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\consultas\detalleproductos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7695" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Depositos" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -172,19 +177,22 @@
   </si>
   <si>
     <t>Consultas</t>
+  </si>
+  <si>
+    <t>testing10</t>
+  </si>
+  <si>
+    <t>999999</t>
+  </si>
+  <si>
+    <t>*6878</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -208,158 +216,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,194 +248,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -594,254 +272,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -854,66 +290,22 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="Normal 2" xfId="32"/>
-    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="40" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="41" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="43" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="44" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="45" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="46" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="47" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="48" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="49" builtinId="52"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1171,19 +563,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="11.125" customWidth="1"/>
     <col min="2" max="6" width="14.375" customWidth="1"/>
@@ -1327,7 +719,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1342,27 +734,32 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="11.125" customWidth="1"/>
     <col min="2" max="6" width="14.375" customWidth="1"/>
@@ -1460,7 +857,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1474,7 +871,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1489,27 +886,32 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:N2"/>
+      <selection sqref="A1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="11.125" customWidth="1"/>
     <col min="2" max="6" width="14.375" customWidth="1"/>
@@ -1608,7 +1010,7 @@
         <v>29281023956</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
@@ -1622,7 +1024,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1637,27 +1039,32 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
@@ -1736,26 +1143,31 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J2">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="11.125" customWidth="1"/>
     <col min="2" max="6" width="14.375" customWidth="1"/>
@@ -1853,21 +1265,51 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12">
+    <row r="3" spans="1:14">
+      <c r="A3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="5"/>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -1882,27 +1324,32 @@
       <c r="L4" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J4">
-      <formula1>Listas!$A$2:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Listas!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:J4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.625" customWidth="1"/>
     <col min="2" max="2" width="14.875" customWidth="1"/>
@@ -1952,7 +1399,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>46</v>
       </c>
@@ -1960,23 +1407,22 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="1:4">
       <c r="B5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="1:4">
       <c r="B6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>